<commit_message>
feat: :sparkles: dialog, useModal, deleting branches, creating a model by default, changing xlsx template
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">🧑‍⚕️</t>
   </si>
   <si>
-    <t xml:space="preserve">Infirimière</t>
+    <t xml:space="preserve">Infirmière</t>
   </si>
   <si>
     <t xml:space="preserve">Diéteticien</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Activités physiques</t>
   </si>
   <si>
-    <t xml:space="preserve">🏋️</t>
+    <t xml:space="preserve">🏃</t>
   </si>
   <si>
     <t xml:space="preserve">Médicaments</t>
@@ -259,8 +259,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,289 +291,289 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="17.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>